<commit_message>
✨ feat(transactions): Implement transaction deletion functionality and update user ID in bank accounts
</commit_message>
<xml_diff>
--- a/aiconomy-client/src/main/resources/assets/transactions.xlsx
+++ b/aiconomy-client/src/main/resources/assets/transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp2022213665\IdeaProjects\aiconomy\aiconomy-client\src\main\resources\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B7B74E-6FDF-4B5E-B966-05A3BA214C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AC5F7F-7ACF-4895-86FF-69882A49CF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="8265" windowWidth="24945" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15780" yWindow="6975" windowWidth="24945" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -61,9 +61,6 @@
     <t>remark</t>
   </si>
   <si>
-    <t>12345</t>
-  </si>
-  <si>
     <t>2025-04-16T10:30:00</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>成功</t>
   </si>
   <si>
-    <t>7890</t>
-  </si>
-  <si>
     <t>acc1</t>
   </si>
   <si>
@@ -88,88 +82,73 @@
     <t>购买iPhone 15</t>
   </si>
   <si>
-    <t>12346</t>
-  </si>
-  <si>
     <t>2025-04-17T12:45:00</t>
   </si>
   <si>
     <t>MacBook Pro</t>
   </si>
   <si>
-    <t>7891</t>
-  </si>
-  <si>
     <t>acc2</t>
   </si>
   <si>
     <t>收到MacBook款项</t>
   </si>
   <si>
-    <t>12347</t>
-  </si>
-  <si>
     <t>2025-04-18T09:00:00</t>
   </si>
   <si>
     <t>待支付</t>
   </si>
   <si>
-    <t>7892</t>
-  </si>
-  <si>
     <t>购买耳机</t>
   </si>
   <si>
-    <t>12348</t>
-  </si>
-  <si>
     <t>2025-04-19T15:00:00</t>
   </si>
   <si>
-    <t>7893</t>
+    <t>expense</t>
   </si>
   <si>
     <t>Shopping</t>
+  </si>
+  <si>
+    <t>WeChat Pay</t>
+  </si>
+  <si>
+    <t>AliPay</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>Earphone</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>收到电视款项</t>
+  </si>
+  <si>
+    <t>599.99</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>expense</t>
+    <t>1299.00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WeChat Pay</t>
+    <t>29.99</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AliPay</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>expense</t>
-  </si>
-  <si>
-    <t>Credit Card</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earphone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Television</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>收到电视款项</t>
+    <t>499.00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -215,8 +194,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -556,7 +538,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -617,167 +599,167 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>12345</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2">
-        <v>599.99</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2">
+        <v>7890</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>12346</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>7891</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3">
-        <v>1299</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>12347</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4">
-        <v>29.99</v>
+      <c r="G4" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>7892</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
+      <c r="A5">
+        <v>12348</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5">
-        <v>499</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
       <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>7893</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>